<commit_message>
Big Ol late edit
</commit_message>
<xml_diff>
--- a/Stimuli/MDMK.xlsx
+++ b/Stimuli/MDMK.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1948" uniqueCount="608">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1948" uniqueCount="614">
   <si>
     <t>item</t>
   </si>
@@ -1916,6 +1916,24 @@
   </si>
   <si>
     <t xml:space="preserve">Benjamin, the mechanic, had only recently arrived on the island. He had been called there on the behest of his friend Allan, who was also a mechanic, in order to fix the islands lighthouse. Benjamin was not as good of a mechanic as Allan but they were sure to make a good team nonetheless. After a long day of trying to repair the lighthouse there was still much work to do to get it working. Allan decided to call for help. Susan, who also lived on the Island, was not as good of a mechanic as Allan but surely the three of them would complete the work faster than just the two of them. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The office wasn’t really much of an office, it was more of a warehouse with desks. Somewhere to the left of the office managers desk stood a water cooler. She had placed it there so that she could keep an eye on her underlings so that they wouldn’t be tempted to chat away the whole working day. The air conditioner had recently broken making the office hellishly hot. The manager had placed an order for a large fan so that it would be at least somewhat cooler. She’d made sure that it would be placed somewhere to the right of the water cooler so that she could keep an eye on it and control the settings if she needed to. </t>
+  </si>
+  <si>
+    <t>Three difficult custom jobs had come to Daren's workshop in one day. This was most unusual, most of the time he struggled to get 3 jobs in one week, let alone in a day. He was going to need some of his friends to help him. Daren was a much better metal worker than his friend Steve but he needed his help none the less. The two were good friends and the work was sure to go smoothly with them working together. Toby was relatively new to the trade but was a good worker none the less, he obviously wasn’t as good as Daren but he would still be a valuable asset while working on the 3 jobs.</t>
+  </si>
+  <si>
+    <t>The office wasn’t really much of an office, it was more of a warehouse with desks. Somewhere to the left of the office managers desk stood a water cooler. She had placed it there so that she could keep an eye on her underlings so that they wouldn’t be tempted to chat away the whole working day. The air conditioner had recently broken making the office hellishly hot. The manager had placed an order for a large fan so that it would be at least somewhat cooler. She’d made sure that it would be placed somewhere to the left of the water cooler so that she could keep an eye on it and control the settings if she needed to.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Three difficult custom jobs had come to Daren's workshop in one day. This was most unusual, most of the time he struggled to get 3 jobs in one week, let alone in a day. He was going to need his some of his friends to help him. Daren was a much better metal worker than his friend Steve but he needed his help none the less. The two were good friends and the work was sure to go smoothly with them working together. Toby was relatively new to the trade but was a good worker none the less, he was obviously better than Daren and he would be a valuable asset while working on the 3 jobs. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alfred McMurphy had managed the pub ever since his father had retired several years ago. It was a family operation and always had been. Frank McMurphy wasn’t as popular with the patrons as his brother Alfred but they liked him well enough. They were all popular when they served the drinks and listened to patrons woes. Susan McMurphy also worked at the pub and was a lot more popular as her brother Alfred.  It didn't matter of course, to the McMurphy's Family always came first. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alfred McMurphy had managed the pub ever since his father had retired several years ago. It was a family operation and always had been. Frank McMurphy wasn’t as popular with the patrons as his brother Alfred but they liked him well enough. They were all popular when they served the drinks and listened to patrons woes. Susan McMurphy also worked at the pub and was also not as popular as her brother Alfred. It didn't matter of course, to the McMurphy's Family always came first. </t>
   </si>
 </sst>
 </file>
@@ -2319,8 +2337,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BQ202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AZ1" workbookViewId="0">
-      <selection activeCell="BP51" sqref="BP51"/>
+    <sheetView tabSelected="1" topLeftCell="AZ13" workbookViewId="0">
+      <selection activeCell="BQ20" sqref="BQ20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5200,7 +5218,7 @@
         <v>137</v>
       </c>
       <c r="BP14" s="22" t="s">
-        <v>577</v>
+        <v>608</v>
       </c>
       <c r="BQ14" s="22" t="s">
         <v>403</v>
@@ -5409,7 +5427,7 @@
         <v>364</v>
       </c>
       <c r="BQ15" s="22" t="s">
-        <v>372</v>
+        <v>609</v>
       </c>
     </row>
     <row r="16" spans="1:69" x14ac:dyDescent="0.25">
@@ -6439,7 +6457,7 @@
         <v>89</v>
       </c>
       <c r="BQ20" s="22" t="s">
-        <v>375</v>
+        <v>613</v>
       </c>
     </row>
     <row r="21" spans="1:69" x14ac:dyDescent="0.25">
@@ -8682,7 +8700,7 @@
         <v>352</v>
       </c>
       <c r="BP39" s="22" t="s">
-        <v>578</v>
+        <v>610</v>
       </c>
       <c r="BQ39" s="22" t="s">
         <v>404</v>
@@ -8774,7 +8792,7 @@
         <v>365</v>
       </c>
       <c r="BQ40" s="22" t="s">
-        <v>565</v>
+        <v>611</v>
       </c>
     </row>
     <row r="41" spans="1:69" x14ac:dyDescent="0.25">
@@ -9219,7 +9237,7 @@
         <v>115</v>
       </c>
       <c r="BQ45" s="22" t="s">
-        <v>376</v>
+        <v>612</v>
       </c>
     </row>
     <row r="46" spans="1:69" x14ac:dyDescent="0.25">
@@ -20791,7 +20809,7 @@
         <v xml:space="preserve">The Farmer is standing by the rusty tractor facing it, which way does he need to go to get to his quad bike? </v>
       </c>
       <c r="G195" s="21" t="str">
-        <f t="shared" ref="G194:G201" ca="1" si="68">INDIRECT("AD"&amp;A194)</f>
+        <f t="shared" ref="G195:G201" ca="1" si="68">INDIRECT("AD"&amp;A194)</f>
         <v>Right</v>
       </c>
       <c r="H195" s="21" t="str">

</xml_diff>

<commit_message>
Missing text analysis numbers edit
</commit_message>
<xml_diff>
--- a/Stimuli/MDMK.xlsx
+++ b/Stimuli/MDMK.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3897" uniqueCount="839">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3897" uniqueCount="840">
   <si>
     <t>item</t>
   </si>
@@ -2579,6 +2579,9 @@
   </si>
   <si>
     <t xml:space="preserve">There are a few teams hoping to find Archaeological evidence of Dogger bank settlements that operate in the north sea. The Norwegians have much more funding than the British. Their equipment is proof of this as it's some of the most modern equipment on the market. This didn't mean that anyone was actively working against each other though. As in all sciences, working together is key. The Danish team also have less funding than the Norwegians but they still share their findings with everyone just as the British do. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A tax investigation is launched that will assess work place bonuses. Who has received the biggest bonus out of Lucy and Belinda? </t>
   </si>
 </sst>
 </file>
@@ -3019,7 +3022,7 @@
   <dimension ref="A1:CJ209"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="P1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AH21" sqref="AH21"/>
+      <selection activeCell="AH15" sqref="AH15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6415,7 +6418,7 @@
         <v>3</v>
       </c>
       <c r="AH15" s="1" t="s">
-        <v>169</v>
+        <v>839</v>
       </c>
       <c r="AI15" s="3" t="s">
         <v>305</v>
@@ -6471,7 +6474,7 @@
       </c>
       <c r="AY15" s="10" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">A tax investigation is launched that will assess work place bonuses. Who has received the biggest bonus out of Lucy and Linda? </v>
+        <v xml:space="preserve">A tax investigation is launched that will assess work place bonuses. Who has received the biggest bonus out of Lucy and Belinda? </v>
       </c>
       <c r="AZ15" s="9" t="str">
         <f t="shared" si="5"/>
@@ -16503,7 +16506,7 @@
       </c>
       <c r="F114" s="3" t="str">
         <f ca="1">INDIRECT("AH"&amp;A114)</f>
-        <v xml:space="preserve">A tax investigation is launched that will assess work place bonuses. Who has received the biggest bonus out of Lucy and Linda? </v>
+        <v xml:space="preserve">A tax investigation is launched that will assess work place bonuses. Who has received the biggest bonus out of Lucy and Belinda? </v>
       </c>
       <c r="G114" s="3" t="str">
         <f ca="1">INDIRECT("AI"&amp;A114)</f>
@@ -16582,7 +16585,7 @@
       </c>
       <c r="F115" s="3" t="str">
         <f ca="1">INDIRECT("AH"&amp;A115)</f>
-        <v xml:space="preserve">A tax investigation is launched that will assess work place bonuses. Who has received the biggest bonus out of Lucy and Linda? </v>
+        <v xml:space="preserve">A tax investigation is launched that will assess work place bonuses. Who has received the biggest bonus out of Lucy and Belinda? </v>
       </c>
       <c r="G115" s="3" t="str">
         <f ca="1">INDIRECT("AI"&amp;A115)</f>
@@ -16661,7 +16664,7 @@
       </c>
       <c r="F116" s="3" t="str">
         <f ca="1">INDIRECT("AH"&amp;A116)</f>
-        <v xml:space="preserve">A tax investigation is launched that will assess work place bonuses. Who has received the biggest bonus out of Lucy and Linda? </v>
+        <v xml:space="preserve">A tax investigation is launched that will assess work place bonuses. Who has received the biggest bonus out of Lucy and Belinda? </v>
       </c>
       <c r="G116" s="3" t="str">
         <f ca="1">INDIRECT("AI"&amp;A116)</f>
@@ -16740,7 +16743,7 @@
       </c>
       <c r="F117" s="3" t="str">
         <f ca="1">INDIRECT("AH"&amp;A117)</f>
-        <v xml:space="preserve">A tax investigation is launched that will assess work place bonuses. Who has received the biggest bonus out of Lucy and Linda? </v>
+        <v xml:space="preserve">A tax investigation is launched that will assess work place bonuses. Who has received the biggest bonus out of Lucy and Belinda? </v>
       </c>
       <c r="G117" s="3" t="str">
         <f ca="1">INDIRECT("AI"&amp;A117)</f>
@@ -16839,7 +16842,7 @@
       </c>
       <c r="K118" s="3" t="str">
         <f ca="1">INDIRECT("AH"&amp;A118)</f>
-        <v xml:space="preserve">A tax investigation is launched that will assess work place bonuses. Who has received the biggest bonus out of Lucy and Linda? </v>
+        <v xml:space="preserve">A tax investigation is launched that will assess work place bonuses. Who has received the biggest bonus out of Lucy and Belinda? </v>
       </c>
       <c r="L118" s="3" t="str">
         <f ca="1">INDIRECT("AI"&amp;A118)</f>
@@ -16918,7 +16921,7 @@
       </c>
       <c r="K119" s="3" t="str">
         <f ca="1">INDIRECT("AH"&amp;A119)</f>
-        <v xml:space="preserve">A tax investigation is launched that will assess work place bonuses. Who has received the biggest bonus out of Lucy and Linda? </v>
+        <v xml:space="preserve">A tax investigation is launched that will assess work place bonuses. Who has received the biggest bonus out of Lucy and Belinda? </v>
       </c>
       <c r="L119" s="3" t="str">
         <f ca="1">INDIRECT("AI"&amp;A119)</f>
@@ -16997,7 +17000,7 @@
       </c>
       <c r="K120" s="3" t="str">
         <f ca="1">INDIRECT("AH"&amp;A120)</f>
-        <v xml:space="preserve">A tax investigation is launched that will assess work place bonuses. Who has received the biggest bonus out of Lucy and Linda? </v>
+        <v xml:space="preserve">A tax investigation is launched that will assess work place bonuses. Who has received the biggest bonus out of Lucy and Belinda? </v>
       </c>
       <c r="L120" s="3" t="str">
         <f ca="1">INDIRECT("AI"&amp;A120)</f>
@@ -17076,7 +17079,7 @@
       </c>
       <c r="K121" s="3" t="str">
         <f ca="1">INDIRECT("AH"&amp;A121)</f>
-        <v xml:space="preserve">A tax investigation is launched that will assess work place bonuses. Who has received the biggest bonus out of Lucy and Linda? </v>
+        <v xml:space="preserve">A tax investigation is launched that will assess work place bonuses. Who has received the biggest bonus out of Lucy and Belinda? </v>
       </c>
       <c r="L121" s="3" t="str">
         <f ca="1">INDIRECT("AI"&amp;A121)</f>

</xml_diff>

<commit_message>
So can work from home without chunky asc files
</commit_message>
<xml_diff>
--- a/Stimuli/MDMK.xlsx
+++ b/Stimuli/MDMK.xlsx
@@ -3021,14 +3021,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CJ209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AH15" sqref="AH15"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AQ19" sqref="AQ19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="10" max="10" width="28.42578125" style="3" customWidth="1"/>
     <col min="15" max="15" width="28.42578125" style="3" customWidth="1"/>
+    <col min="51" max="51" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:88" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Accidental re-upload from a change of folders
</commit_message>
<xml_diff>
--- a/Stimuli/MDMK.xlsx
+++ b/Stimuli/MDMK.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3897" uniqueCount="840">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3897" uniqueCount="843">
   <si>
     <t>item</t>
   </si>
@@ -2582,6 +2582,15 @@
   </si>
   <si>
     <t>The Kingsley hills tourism board were looking to build a museum to display the archaeological findings of the area. The board were looking for local businesses to co-fund the project. Farmer Jack's farm shop was eager to fund the project. However, Farmer Jack's were not as wealthy as The Pepper Mills Hotel. So couldn't offer as much money as them. The local bus company also wanted to co-fund the project. They were even wealthier than The Pepper Mills hotel. The tourism board were sure that they would have all they needed to build the museum.</t>
+  </si>
+  <si>
+    <t>Which of the charity running teams is most likely to finish the marathon first?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The town of Rockport boasted three major events that always drew in large amounts of crowds. There were also a few smaller events for locals in the summer. The Folk music festival drew in a much larger crowd than the Rockport Grand Prix. Both were important sources of income in the town. The Sailing festival was also more popular than the Rockport Grand Prix but this didn't matter to the townsfolk. Rockport was one of the most up and coming towns in the area. The yearly events were beginning to draw in crowds from further and further afield. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The town of Rockport boasted three major events that always drew in large amounts of crowds. There were also a few smaller events for locals in the summer. The Folk music festival drew in a much larger crowd than the Rockport Grand Prix. Both were important sources of income in the town. The Sailing festival was less popular than the Rockport Grand Prix but this didn't matter to the townsfolk. Rockport was one of the most up and coming towns in the area. The yearly events were beginning to draw in crowds from further and further afield. </t>
   </si>
 </sst>
 </file>
@@ -3022,7 +3031,7 @@
   <dimension ref="A1:CJ209"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="W18" sqref="W18"/>
+      <selection activeCell="X17" sqref="X17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4759,7 +4768,7 @@
         <v>121</v>
       </c>
       <c r="AC8" s="1" t="s">
-        <v>432</v>
+        <v>840</v>
       </c>
       <c r="AD8" s="3" t="s">
         <v>268</v>
@@ -4811,7 +4820,7 @@
       </c>
       <c r="AT8" s="8" t="str">
         <f t="shared" si="2"/>
-        <v>Which of the chairty running teams is most likely to finish the marathon first?</v>
+        <v>Which of the charity running teams is most likely to finish the marathon first?</v>
       </c>
       <c r="AU8" s="9" t="str">
         <f t="shared" si="3"/>
@@ -6856,10 +6865,10 @@
         <v>17</v>
       </c>
       <c r="W17" s="19" t="s">
-        <v>215</v>
+        <v>841</v>
       </c>
       <c r="X17" s="19" t="s">
-        <v>214</v>
+        <v>842</v>
       </c>
       <c r="Y17" s="19" t="s">
         <v>801</v>
@@ -7225,7 +7234,7 @@
       </c>
       <c r="BQ18" s="4" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">The town of Rockport boasted three major events that always drew in large amounts of crowds. There were also a few smaller events for locals in the summer. The Folk music festival drew in a much larger crowd than the Rockport Grand Prix. Both were important sources of income in the town. The Sailing festival was also more popular the Rockport Grand Prix but this didn't matter to the townsfolk. Rockport was one of the most up and coming towns in the area. The yearly events were beginning to draw in crowds from further and further afield. </v>
+        <v xml:space="preserve">The town of Rockport boasted three major events that always drew in large amounts of crowds. There were also a few smaller events for locals in the summer. The Folk music festival drew in a much larger crowd than the Rockport Grand Prix. Both were important sources of income in the town. The Sailing festival was also more popular than the Rockport Grand Prix but this didn't matter to the townsfolk. Rockport was one of the most up and coming towns in the area. The yearly events were beginning to draw in crowds from further and further afield. </v>
       </c>
       <c r="BV18" s="1"/>
       <c r="BW18" s="19"/>
@@ -10892,7 +10901,7 @@
       </c>
       <c r="BQ44" s="19" t="str">
         <f t="shared" si="54"/>
-        <v xml:space="preserve">The town of Rockport boasted three major events that always drew in large amounts of crowds. There were also a few smaller events for locals in the summer. The Folk music festival drew in a much larger crowd than the Rockport Grand Prix. Both were important sources of income in the town. The Sailing festival was less popular the Rockport Grand Prix but this didn't matter to the townsfolk. Rockport was one of the most up and coming towns in the area. The yearly events were beginning to draw in crowds from further and further afield. </v>
+        <v xml:space="preserve">The town of Rockport boasted three major events that always drew in large amounts of crowds. There were also a few smaller events for locals in the summer. The Folk music festival drew in a much larger crowd than the Rockport Grand Prix. Both were important sources of income in the town. The Sailing festival was less popular than the Rockport Grand Prix but this didn't matter to the townsfolk. Rockport was one of the most up and coming towns in the area. The yearly events were beginning to draw in crowds from further and further afield. </v>
       </c>
     </row>
     <row r="45" spans="1:69" x14ac:dyDescent="0.25">
@@ -12102,7 +12111,7 @@
       </c>
       <c r="K58" s="3" t="str">
         <f ca="1">INDIRECT("AC"&amp;A58)</f>
-        <v>Which of the chairty running teams is most likely to finish the marathon first?</v>
+        <v>Which of the charity running teams is most likely to finish the marathon first?</v>
       </c>
       <c r="L58" s="3" t="str">
         <f ca="1">INDIRECT("AD"&amp;A58)</f>
@@ -12182,7 +12191,7 @@
       </c>
       <c r="K59" s="3" t="str">
         <f ca="1">INDIRECT("AC"&amp;A59)</f>
-        <v>Which of the chairty running teams is most likely to finish the marathon first?</v>
+        <v>Which of the charity running teams is most likely to finish the marathon first?</v>
       </c>
       <c r="L59" s="3" t="str">
         <f ca="1">INDIRECT("AD"&amp;A59)</f>
@@ -12261,7 +12270,7 @@
       </c>
       <c r="K60" s="3" t="str">
         <f ca="1">INDIRECT("AC"&amp;A60)</f>
-        <v>Which of the chairty running teams is most likely to finish the marathon first?</v>
+        <v>Which of the charity running teams is most likely to finish the marathon first?</v>
       </c>
       <c r="L60" s="3" t="str">
         <f ca="1">INDIRECT("AD"&amp;A60)</f>
@@ -12340,7 +12349,7 @@
       </c>
       <c r="K61" s="3" t="str">
         <f ca="1">INDIRECT("AC"&amp;A61)</f>
-        <v>Which of the chairty running teams is most likely to finish the marathon first?</v>
+        <v>Which of the charity running teams is most likely to finish the marathon first?</v>
       </c>
       <c r="L61" s="3" t="str">
         <f ca="1">INDIRECT("AD"&amp;A61)</f>
@@ -12399,7 +12408,7 @@
       </c>
       <c r="F62" s="3" t="str">
         <f ca="1">INDIRECT("AC"&amp;A62)</f>
-        <v>Which of the chairty running teams is most likely to finish the marathon first?</v>
+        <v>Which of the charity running teams is most likely to finish the marathon first?</v>
       </c>
       <c r="G62" s="3" t="str">
         <f ca="1">INDIRECT("AD"&amp;A61)</f>
@@ -12478,7 +12487,7 @@
       </c>
       <c r="F63" s="3" t="str">
         <f ca="1">INDIRECT("AC"&amp;A63)</f>
-        <v>Which of the chairty running teams is most likely to finish the marathon first?</v>
+        <v>Which of the charity running teams is most likely to finish the marathon first?</v>
       </c>
       <c r="G63" s="3" t="str">
         <f ca="1">INDIRECT("AD"&amp;A62)</f>
@@ -12557,7 +12566,7 @@
       </c>
       <c r="F64" s="3" t="str">
         <f ca="1">INDIRECT("AC"&amp;A64)</f>
-        <v>Which of the chairty running teams is most likely to finish the marathon first?</v>
+        <v>Which of the charity running teams is most likely to finish the marathon first?</v>
       </c>
       <c r="G64" s="3" t="str">
         <f ca="1">INDIRECT("AD"&amp;A63)</f>
@@ -12636,7 +12645,7 @@
       </c>
       <c r="F65" s="3" t="str">
         <f ca="1">INDIRECT("AC"&amp;A65)</f>
-        <v>Which of the chairty running teams is most likely to finish the marathon first?</v>
+        <v>Which of the charity running teams is most likely to finish the marathon first?</v>
       </c>
       <c r="G65" s="3" t="str">
         <f ca="1">INDIRECT("AD"&amp;A64)</f>
@@ -17759,7 +17768,7 @@
       </c>
       <c r="C130" s="3" t="str">
         <f ca="1">INDIRECT("W"&amp;A130)</f>
-        <v xml:space="preserve">The town of Rockport boasted three major events that always drew in large amounts of crowds. There were also a few smaller events for locals in the summer. The Folk music festival drew in a much larger crowd than the Rockport Grand Prix. Both were important sources of income in the town. The Sailing festival was also more popular the Rockport Grand Prix but this didn't matter to the townsfolk. Rockport was one of the most up and coming towns in the area. The yearly events were beginning to draw in crowds from further and further afield. </v>
+        <v xml:space="preserve">The town of Rockport boasted three major events that always drew in large amounts of crowds. There were also a few smaller events for locals in the summer. The Folk music festival drew in a much larger crowd than the Rockport Grand Prix. Both were important sources of income in the town. The Sailing festival was also more popular than the Rockport Grand Prix but this didn't matter to the townsfolk. Rockport was one of the most up and coming towns in the area. The yearly events were beginning to draw in crowds from further and further afield. </v>
       </c>
       <c r="D130" s="3" t="str">
         <f ca="1">INDIRECT("Y"&amp;A130)</f>
@@ -17767,7 +17776,7 @@
       </c>
       <c r="E130" s="3" t="str">
         <f t="shared" ca="1" si="142"/>
-        <v xml:space="preserve">The town of Rockport boasted three major events that always drew in large amounts of crowds. There were also a few smaller events for locals in the summer. The Folk music festival drew in a much larger crowd than the Rockport Grand Prix. Both were important sources of income in the town. The Sailing festival was also more popular the Rockport Grand Prix but this didn't matter to the townsfolk. Rockport was one of the most up and coming towns in the area. The yearly events were beginning to draw in crowds from further and further afield. The Rockport Grand Prix was anything but grand. It was a go-cart race for the under 15s and none of the carts could go about 30 miles per hour. The Blue team was one of the best in Rockport and was currently in front of the Red team. The coaches were happy about this as they had to beat the Red and Green team to qualify for the finals. The Green team were also ahead of the Reds. The Grand Prix was always a popular event in Rockport and would draw in onlookers from miles around. </v>
+        <v xml:space="preserve">The town of Rockport boasted three major events that always drew in large amounts of crowds. There were also a few smaller events for locals in the summer. The Folk music festival drew in a much larger crowd than the Rockport Grand Prix. Both were important sources of income in the town. The Sailing festival was also more popular than the Rockport Grand Prix but this didn't matter to the townsfolk. Rockport was one of the most up and coming towns in the area. The yearly events were beginning to draw in crowds from further and further afield. The Rockport Grand Prix was anything but grand. It was a go-cart race for the under 15s and none of the carts could go about 30 miles per hour. The Blue team was one of the best in Rockport and was currently in front of the Red team. The coaches were happy about this as they had to beat the Red and Green team to qualify for the finals. The Green team were also ahead of the Reds. The Grand Prix was always a popular event in Rockport and would draw in onlookers from miles around. </v>
       </c>
       <c r="F130" s="3" t="str">
         <f ca="1">INDIRECT("AH"&amp;A130)</f>
@@ -17838,7 +17847,7 @@
       </c>
       <c r="C131" s="3" t="str">
         <f ca="1">INDIRECT("X"&amp;A131)</f>
-        <v xml:space="preserve">The town of Rockport boasted three major events that always drew in large amounts of crowds. There were also a few smaller events for locals in the summer. The Folk music festival drew in a much larger crowd than the Rockport Grand Prix. Both were important sources of income in the town. The Sailing festival was less popular the Rockport Grand Prix but this didn't matter to the townsfolk. Rockport was one of the most up and coming towns in the area. The yearly events were beginning to draw in crowds from further and further afield. </v>
+        <v xml:space="preserve">The town of Rockport boasted three major events that always drew in large amounts of crowds. There were also a few smaller events for locals in the summer. The Folk music festival drew in a much larger crowd than the Rockport Grand Prix. Both were important sources of income in the town. The Sailing festival was less popular than the Rockport Grand Prix but this didn't matter to the townsfolk. Rockport was one of the most up and coming towns in the area. The yearly events were beginning to draw in crowds from further and further afield. </v>
       </c>
       <c r="D131" s="3" t="str">
         <f ca="1">INDIRECT("Z"&amp;A131)</f>
@@ -17846,7 +17855,7 @@
       </c>
       <c r="E131" s="3" t="str">
         <f t="shared" ca="1" si="142"/>
-        <v xml:space="preserve">The town of Rockport boasted three major events that always drew in large amounts of crowds. There were also a few smaller events for locals in the summer. The Folk music festival drew in a much larger crowd than the Rockport Grand Prix. Both were important sources of income in the town. The Sailing festival was less popular the Rockport Grand Prix but this didn't matter to the townsfolk. Rockport was one of the most up and coming towns in the area. The yearly events were beginning to draw in crowds from further and further afield. The Rockport Grand Prix was anything but grand. It was a go-cart race for the under 15s and none of the carts could go about 30 miles per hour. The Blue team was one of the best in Rockport and was currently in front of the Red team. The coaches were happy about this as they had to beat the Red and Green team to qualify for the finals. The Green team were behind of the Reds. The Grand Prix was always a popular event in Rockport and would draw in onlookers from miles around. </v>
+        <v xml:space="preserve">The town of Rockport boasted three major events that always drew in large amounts of crowds. There were also a few smaller events for locals in the summer. The Folk music festival drew in a much larger crowd than the Rockport Grand Prix. Both were important sources of income in the town. The Sailing festival was less popular than the Rockport Grand Prix but this didn't matter to the townsfolk. Rockport was one of the most up and coming towns in the area. The yearly events were beginning to draw in crowds from further and further afield. The Rockport Grand Prix was anything but grand. It was a go-cart race for the under 15s and none of the carts could go about 30 miles per hour. The Blue team was one of the best in Rockport and was currently in front of the Red team. The coaches were happy about this as they had to beat the Red and Green team to qualify for the finals. The Green team were behind of the Reds. The Grand Prix was always a popular event in Rockport and would draw in onlookers from miles around. </v>
       </c>
       <c r="F131" s="3" t="str">
         <f ca="1">INDIRECT("AH"&amp;A131)</f>
@@ -17917,7 +17926,7 @@
       </c>
       <c r="C132" s="3" t="str">
         <f ca="1">INDIRECT("W"&amp;A132)</f>
-        <v xml:space="preserve">The town of Rockport boasted three major events that always drew in large amounts of crowds. There were also a few smaller events for locals in the summer. The Folk music festival drew in a much larger crowd than the Rockport Grand Prix. Both were important sources of income in the town. The Sailing festival was also more popular the Rockport Grand Prix but this didn't matter to the townsfolk. Rockport was one of the most up and coming towns in the area. The yearly events were beginning to draw in crowds from further and further afield. </v>
+        <v xml:space="preserve">The town of Rockport boasted three major events that always drew in large amounts of crowds. There were also a few smaller events for locals in the summer. The Folk music festival drew in a much larger crowd than the Rockport Grand Prix. Both were important sources of income in the town. The Sailing festival was also more popular than the Rockport Grand Prix but this didn't matter to the townsfolk. Rockport was one of the most up and coming towns in the area. The yearly events were beginning to draw in crowds from further and further afield. </v>
       </c>
       <c r="D132" s="3" t="str">
         <f ca="1">INDIRECT("Z"&amp;A132)</f>
@@ -17925,7 +17934,7 @@
       </c>
       <c r="E132" s="3" t="str">
         <f t="shared" ca="1" si="142"/>
-        <v xml:space="preserve">The town of Rockport boasted three major events that always drew in large amounts of crowds. There were also a few smaller events for locals in the summer. The Folk music festival drew in a much larger crowd than the Rockport Grand Prix. Both were important sources of income in the town. The Sailing festival was also more popular the Rockport Grand Prix but this didn't matter to the townsfolk. Rockport was one of the most up and coming towns in the area. The yearly events were beginning to draw in crowds from further and further afield. The Rockport Grand Prix was anything but grand. It was a go-cart race for the under 15s and none of the carts could go about 30 miles per hour. The Blue team was one of the best in Rockport and was currently in front of the Red team. The coaches were happy about this as they had to beat the Red and Green team to qualify for the finals. The Green team were behind of the Reds. The Grand Prix was always a popular event in Rockport and would draw in onlookers from miles around. </v>
+        <v xml:space="preserve">The town of Rockport boasted three major events that always drew in large amounts of crowds. There were also a few smaller events for locals in the summer. The Folk music festival drew in a much larger crowd than the Rockport Grand Prix. Both were important sources of income in the town. The Sailing festival was also more popular than the Rockport Grand Prix but this didn't matter to the townsfolk. Rockport was one of the most up and coming towns in the area. The yearly events were beginning to draw in crowds from further and further afield. The Rockport Grand Prix was anything but grand. It was a go-cart race for the under 15s and none of the carts could go about 30 miles per hour. The Blue team was one of the best in Rockport and was currently in front of the Red team. The coaches were happy about this as they had to beat the Red and Green team to qualify for the finals. The Green team were behind of the Reds. The Grand Prix was always a popular event in Rockport and would draw in onlookers from miles around. </v>
       </c>
       <c r="F132" s="3" t="str">
         <f ca="1">INDIRECT("AH"&amp;A132)</f>
@@ -17996,7 +18005,7 @@
       </c>
       <c r="C133" s="3" t="str">
         <f ca="1">INDIRECT("X"&amp;A133)</f>
-        <v xml:space="preserve">The town of Rockport boasted three major events that always drew in large amounts of crowds. There were also a few smaller events for locals in the summer. The Folk music festival drew in a much larger crowd than the Rockport Grand Prix. Both were important sources of income in the town. The Sailing festival was less popular the Rockport Grand Prix but this didn't matter to the townsfolk. Rockport was one of the most up and coming towns in the area. The yearly events were beginning to draw in crowds from further and further afield. </v>
+        <v xml:space="preserve">The town of Rockport boasted three major events that always drew in large amounts of crowds. There were also a few smaller events for locals in the summer. The Folk music festival drew in a much larger crowd than the Rockport Grand Prix. Both were important sources of income in the town. The Sailing festival was less popular than the Rockport Grand Prix but this didn't matter to the townsfolk. Rockport was one of the most up and coming towns in the area. The yearly events were beginning to draw in crowds from further and further afield. </v>
       </c>
       <c r="D133" s="3" t="str">
         <f ca="1">INDIRECT("Y"&amp;A133)</f>
@@ -18004,7 +18013,7 @@
       </c>
       <c r="E133" s="3" t="str">
         <f t="shared" ca="1" si="142"/>
-        <v xml:space="preserve">The town of Rockport boasted three major events that always drew in large amounts of crowds. There were also a few smaller events for locals in the summer. The Folk music festival drew in a much larger crowd than the Rockport Grand Prix. Both were important sources of income in the town. The Sailing festival was less popular the Rockport Grand Prix but this didn't matter to the townsfolk. Rockport was one of the most up and coming towns in the area. The yearly events were beginning to draw in crowds from further and further afield. The Rockport Grand Prix was anything but grand. It was a go-cart race for the under 15s and none of the carts could go about 30 miles per hour. The Blue team was one of the best in Rockport and was currently in front of the Red team. The coaches were happy about this as they had to beat the Red and Green team to qualify for the finals. The Green team were also ahead of the Reds. The Grand Prix was always a popular event in Rockport and would draw in onlookers from miles around. </v>
+        <v xml:space="preserve">The town of Rockport boasted three major events that always drew in large amounts of crowds. There were also a few smaller events for locals in the summer. The Folk music festival drew in a much larger crowd than the Rockport Grand Prix. Both were important sources of income in the town. The Sailing festival was less popular than the Rockport Grand Prix but this didn't matter to the townsfolk. Rockport was one of the most up and coming towns in the area. The yearly events were beginning to draw in crowds from further and further afield. The Rockport Grand Prix was anything but grand. It was a go-cart race for the under 15s and none of the carts could go about 30 miles per hour. The Blue team was one of the best in Rockport and was currently in front of the Red team. The coaches were happy about this as they had to beat the Red and Green team to qualify for the finals. The Green team were also ahead of the Reds. The Grand Prix was always a popular event in Rockport and would draw in onlookers from miles around. </v>
       </c>
       <c r="F133" s="3" t="str">
         <f ca="1">INDIRECT("AH"&amp;A133)</f>
@@ -18079,11 +18088,11 @@
       </c>
       <c r="D134" s="3" t="str">
         <f ca="1">INDIRECT("W"&amp;A134)</f>
-        <v xml:space="preserve">The town of Rockport boasted three major events that always drew in large amounts of crowds. There were also a few smaller events for locals in the summer. The Folk music festival drew in a much larger crowd than the Rockport Grand Prix. Both were important sources of income in the town. The Sailing festival was also more popular the Rockport Grand Prix but this didn't matter to the townsfolk. Rockport was one of the most up and coming towns in the area. The yearly events were beginning to draw in crowds from further and further afield. </v>
+        <v xml:space="preserve">The town of Rockport boasted three major events that always drew in large amounts of crowds. There were also a few smaller events for locals in the summer. The Folk music festival drew in a much larger crowd than the Rockport Grand Prix. Both were important sources of income in the town. The Sailing festival was also more popular than the Rockport Grand Prix but this didn't matter to the townsfolk. Rockport was one of the most up and coming towns in the area. The yearly events were beginning to draw in crowds from further and further afield. </v>
       </c>
       <c r="E134" s="3" t="str">
         <f t="shared" ca="1" si="142"/>
-        <v xml:space="preserve">The Rockport Grand Prix was anything but grand. It was a go-cart race for the under 15s and none of the carts could go about 30 miles per hour. The Blue team was one of the best in Rockport and was currently in front of the Red team. The coaches were happy about this as they had to beat the Red and Green team to qualify for the finals. The Green team were also ahead of the Reds. The Grand Prix was always a popular event in Rockport and would draw in onlookers from miles around. The town of Rockport boasted three major events that always drew in large amounts of crowds. There were also a few smaller events for locals in the summer. The Folk music festival drew in a much larger crowd than the Rockport Grand Prix. Both were important sources of income in the town. The Sailing festival was also more popular the Rockport Grand Prix but this didn't matter to the townsfolk. Rockport was one of the most up and coming towns in the area. The yearly events were beginning to draw in crowds from further and further afield. </v>
+        <v xml:space="preserve">The Rockport Grand Prix was anything but grand. It was a go-cart race for the under 15s and none of the carts could go about 30 miles per hour. The Blue team was one of the best in Rockport and was currently in front of the Red team. The coaches were happy about this as they had to beat the Red and Green team to qualify for the finals. The Green team were also ahead of the Reds. The Grand Prix was always a popular event in Rockport and would draw in onlookers from miles around. The town of Rockport boasted three major events that always drew in large amounts of crowds. There were also a few smaller events for locals in the summer. The Folk music festival drew in a much larger crowd than the Rockport Grand Prix. Both were important sources of income in the town. The Sailing festival was also more popular than the Rockport Grand Prix but this didn't matter to the townsfolk. Rockport was one of the most up and coming towns in the area. The yearly events were beginning to draw in crowds from further and further afield. </v>
       </c>
       <c r="F134" s="3" t="str">
         <f ca="1">INDIRECT("AC"&amp;A134)</f>
@@ -18158,11 +18167,11 @@
       </c>
       <c r="D135" s="3" t="str">
         <f ca="1">INDIRECT("X"&amp;A135)</f>
-        <v xml:space="preserve">The town of Rockport boasted three major events that always drew in large amounts of crowds. There were also a few smaller events for locals in the summer. The Folk music festival drew in a much larger crowd than the Rockport Grand Prix. Both were important sources of income in the town. The Sailing festival was less popular the Rockport Grand Prix but this didn't matter to the townsfolk. Rockport was one of the most up and coming towns in the area. The yearly events were beginning to draw in crowds from further and further afield. </v>
+        <v xml:space="preserve">The town of Rockport boasted three major events that always drew in large amounts of crowds. There were also a few smaller events for locals in the summer. The Folk music festival drew in a much larger crowd than the Rockport Grand Prix. Both were important sources of income in the town. The Sailing festival was less popular than the Rockport Grand Prix but this didn't matter to the townsfolk. Rockport was one of the most up and coming towns in the area. The yearly events were beginning to draw in crowds from further and further afield. </v>
       </c>
       <c r="E135" s="3" t="str">
         <f t="shared" ca="1" si="142"/>
-        <v xml:space="preserve">The Rockport Grand Prix was anything but grand. It was a go-cart race for the under 15s and none of the carts could go about 30 miles per hour. The Blue team was one of the best in Rockport and was currently in front of the Red team. The coaches were happy about this as they had to beat the Red and Green team to qualify for the finals. The Green team were behind of the Reds. The Grand Prix was always a popular event in Rockport and would draw in onlookers from miles around. The town of Rockport boasted three major events that always drew in large amounts of crowds. There were also a few smaller events for locals in the summer. The Folk music festival drew in a much larger crowd than the Rockport Grand Prix. Both were important sources of income in the town. The Sailing festival was less popular the Rockport Grand Prix but this didn't matter to the townsfolk. Rockport was one of the most up and coming towns in the area. The yearly events were beginning to draw in crowds from further and further afield. </v>
+        <v xml:space="preserve">The Rockport Grand Prix was anything but grand. It was a go-cart race for the under 15s and none of the carts could go about 30 miles per hour. The Blue team was one of the best in Rockport and was currently in front of the Red team. The coaches were happy about this as they had to beat the Red and Green team to qualify for the finals. The Green team were behind of the Reds. The Grand Prix was always a popular event in Rockport and would draw in onlookers from miles around. The town of Rockport boasted three major events that always drew in large amounts of crowds. There were also a few smaller events for locals in the summer. The Folk music festival drew in a much larger crowd than the Rockport Grand Prix. Both were important sources of income in the town. The Sailing festival was less popular than the Rockport Grand Prix but this didn't matter to the townsfolk. Rockport was one of the most up and coming towns in the area. The yearly events were beginning to draw in crowds from further and further afield. </v>
       </c>
       <c r="F135" s="3" t="str">
         <f ca="1">INDIRECT("AC"&amp;A135)</f>
@@ -18237,11 +18246,11 @@
       </c>
       <c r="D136" s="3" t="str">
         <f ca="1">INDIRECT("X"&amp;A136)</f>
-        <v xml:space="preserve">The town of Rockport boasted three major events that always drew in large amounts of crowds. There were also a few smaller events for locals in the summer. The Folk music festival drew in a much larger crowd than the Rockport Grand Prix. Both were important sources of income in the town. The Sailing festival was less popular the Rockport Grand Prix but this didn't matter to the townsfolk. Rockport was one of the most up and coming towns in the area. The yearly events were beginning to draw in crowds from further and further afield. </v>
+        <v xml:space="preserve">The town of Rockport boasted three major events that always drew in large amounts of crowds. There were also a few smaller events for locals in the summer. The Folk music festival drew in a much larger crowd than the Rockport Grand Prix. Both were important sources of income in the town. The Sailing festival was less popular than the Rockport Grand Prix but this didn't matter to the townsfolk. Rockport was one of the most up and coming towns in the area. The yearly events were beginning to draw in crowds from further and further afield. </v>
       </c>
       <c r="E136" s="3" t="str">
         <f t="shared" ca="1" si="142"/>
-        <v xml:space="preserve">The Rockport Grand Prix was anything but grand. It was a go-cart race for the under 15s and none of the carts could go about 30 miles per hour. The Blue team was one of the best in Rockport and was currently in front of the Red team. The coaches were happy about this as they had to beat the Red and Green team to qualify for the finals. The Green team were also ahead of the Reds. The Grand Prix was always a popular event in Rockport and would draw in onlookers from miles around. The town of Rockport boasted three major events that always drew in large amounts of crowds. There were also a few smaller events for locals in the summer. The Folk music festival drew in a much larger crowd than the Rockport Grand Prix. Both were important sources of income in the town. The Sailing festival was less popular the Rockport Grand Prix but this didn't matter to the townsfolk. Rockport was one of the most up and coming towns in the area. The yearly events were beginning to draw in crowds from further and further afield. </v>
+        <v xml:space="preserve">The Rockport Grand Prix was anything but grand. It was a go-cart race for the under 15s and none of the carts could go about 30 miles per hour. The Blue team was one of the best in Rockport and was currently in front of the Red team. The coaches were happy about this as they had to beat the Red and Green team to qualify for the finals. The Green team were also ahead of the Reds. The Grand Prix was always a popular event in Rockport and would draw in onlookers from miles around. The town of Rockport boasted three major events that always drew in large amounts of crowds. There were also a few smaller events for locals in the summer. The Folk music festival drew in a much larger crowd than the Rockport Grand Prix. Both were important sources of income in the town. The Sailing festival was less popular than the Rockport Grand Prix but this didn't matter to the townsfolk. Rockport was one of the most up and coming towns in the area. The yearly events were beginning to draw in crowds from further and further afield. </v>
       </c>
       <c r="F136" s="3" t="str">
         <f ca="1">INDIRECT("AC"&amp;A136)</f>
@@ -18316,11 +18325,11 @@
       </c>
       <c r="D137" s="3" t="str">
         <f ca="1">INDIRECT("W"&amp;A137)</f>
-        <v xml:space="preserve">The town of Rockport boasted three major events that always drew in large amounts of crowds. There were also a few smaller events for locals in the summer. The Folk music festival drew in a much larger crowd than the Rockport Grand Prix. Both were important sources of income in the town. The Sailing festival was also more popular the Rockport Grand Prix but this didn't matter to the townsfolk. Rockport was one of the most up and coming towns in the area. The yearly events were beginning to draw in crowds from further and further afield. </v>
+        <v xml:space="preserve">The town of Rockport boasted three major events that always drew in large amounts of crowds. There were also a few smaller events for locals in the summer. The Folk music festival drew in a much larger crowd than the Rockport Grand Prix. Both were important sources of income in the town. The Sailing festival was also more popular than the Rockport Grand Prix but this didn't matter to the townsfolk. Rockport was one of the most up and coming towns in the area. The yearly events were beginning to draw in crowds from further and further afield. </v>
       </c>
       <c r="E137" s="3" t="str">
         <f t="shared" ca="1" si="142"/>
-        <v xml:space="preserve">The Rockport Grand Prix was anything but grand. It was a go-cart race for the under 15s and none of the carts could go about 30 miles per hour. The Blue team was one of the best in Rockport and was currently in front of the Red team. The coaches were happy about this as they had to beat the Red and Green team to qualify for the finals. The Green team were behind of the Reds. The Grand Prix was always a popular event in Rockport and would draw in onlookers from miles around. The town of Rockport boasted three major events that always drew in large amounts of crowds. There were also a few smaller events for locals in the summer. The Folk music festival drew in a much larger crowd than the Rockport Grand Prix. Both were important sources of income in the town. The Sailing festival was also more popular the Rockport Grand Prix but this didn't matter to the townsfolk. Rockport was one of the most up and coming towns in the area. The yearly events were beginning to draw in crowds from further and further afield. </v>
+        <v xml:space="preserve">The Rockport Grand Prix was anything but grand. It was a go-cart race for the under 15s and none of the carts could go about 30 miles per hour. The Blue team was one of the best in Rockport and was currently in front of the Red team. The coaches were happy about this as they had to beat the Red and Green team to qualify for the finals. The Green team were behind of the Reds. The Grand Prix was always a popular event in Rockport and would draw in onlookers from miles around. The town of Rockport boasted three major events that always drew in large amounts of crowds. There were also a few smaller events for locals in the summer. The Folk music festival drew in a much larger crowd than the Rockport Grand Prix. Both were important sources of income in the town. The Sailing festival was also more popular than the Rockport Grand Prix but this didn't matter to the townsfolk. Rockport was one of the most up and coming towns in the area. The yearly events were beginning to draw in crowds from further and further afield. </v>
       </c>
       <c r="F137" s="3" t="str">
         <f ca="1">INDIRECT("AC"&amp;A137)</f>

</xml_diff>

<commit_message>
Files Now actually match the ones we use in the lab... FINALLY
</commit_message>
<xml_diff>
--- a/Stimuli/MDMK.xlsx
+++ b/Stimuli/MDMK.xlsx
@@ -2404,9 +2404,6 @@
     <t xml:space="preserve">The A67 highway was the longest road in the county. It spanned almost all of it, and ran over the river Stig. Heading to Innsmouth from Ipswich people had to cross the bridge over the river. Somewhere before this bridge there was a rest stop that offered travellers refreshment. It was a popular place and saw a great many visitors, making it a profitable place to own. A checkpoint had been set up by the police somewhere after the rest stop as there had been reports of drug smuggling in the area. </t>
   </si>
   <si>
-    <t xml:space="preserve">The A67 highway the longest road in the county. It spanned almost all of it, and ran over the river Stig. Heading to Innsmouth from Ipswich people had to cross the bridge over the river. Somewhere before this bridge there was a rest stop that offered travellers refreshment. It was a popular place and saw a great many visitors, making it a profitable place to own. A checkpoint had been set up by the police somewhere before the rest stop as there had been reports of drug smuggling in the area. </t>
-  </si>
-  <si>
     <t>Sunnydale high school was like any high school. The basketball group was quite popular even more popular than the football group. This may have been down to their recent win streak against their rival high school, which had put them on their way to the basketball finals. On another hand the art club had recently also exploded in popularity due to their very successful summer exhibition. Though they were still less popular than the basketball group. Their popularity would influence how many members each group had</t>
   </si>
   <si>
@@ -2591,6 +2588,9 @@
   </si>
   <si>
     <t xml:space="preserve">The town of Rockport boasted three major events that always drew in large amounts of crowds. There were also a few smaller events for locals in the summer. The Folk music festival drew in a much larger crowd than the Rockport Grand Prix. Both were important sources of income in the town. The Sailing festival was less popular than the Rockport Grand Prix but this didn't matter to the townsfolk. Rockport was one of the most up and coming towns in the area. The yearly events were beginning to draw in crowds from further and further afield. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The A67 highway was the longest road in the county. It spanned almost all of it, and ran over the river Stig. Heading to Innsmouth from Ipswich people had to cross the bridge over the river. Somewhere before this bridge there was a rest stop that offered travellers refreshment. It was a popular place and saw a great many visitors, making it a profitable place to own. A checkpoint had been set up by the police somewhere before the rest stop as there had been reports of drug smuggling in the area. </t>
   </si>
 </sst>
 </file>
@@ -3031,7 +3031,7 @@
   <dimension ref="A1:CJ209"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="X17" sqref="X17"/>
+      <selection activeCell="Z24" sqref="Z24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3113,10 +3113,10 @@
         <v>743</v>
       </c>
       <c r="Y1" s="19" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="Z1" s="19" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="AA1" s="3">
         <v>1</v>
@@ -3816,10 +3816,10 @@
         <v>773</v>
       </c>
       <c r="Y4" s="19" t="s">
+        <v>828</v>
+      </c>
+      <c r="Z4" s="19" t="s">
         <v>829</v>
-      </c>
-      <c r="Z4" s="19" t="s">
-        <v>830</v>
       </c>
       <c r="AA4" s="3">
         <v>4</v>
@@ -4289,7 +4289,7 @@
         <v>779</v>
       </c>
       <c r="Z6" s="19" t="s">
-        <v>780</v>
+        <v>842</v>
       </c>
       <c r="AA6" s="3">
         <v>6</v>
@@ -4515,16 +4515,16 @@
         <v>7</v>
       </c>
       <c r="W7" s="19" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="X7" s="19" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="Y7" s="19" t="s">
+        <v>824</v>
+      </c>
+      <c r="Z7" s="19" t="s">
         <v>825</v>
-      </c>
-      <c r="Z7" s="19" t="s">
-        <v>826</v>
       </c>
       <c r="AA7" s="3">
         <v>7</v>
@@ -4750,7 +4750,7 @@
         <v>8</v>
       </c>
       <c r="W8" s="19" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="X8" s="19" t="s">
         <v>755</v>
@@ -4768,7 +4768,7 @@
         <v>121</v>
       </c>
       <c r="AC8" s="1" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="AD8" s="3" t="s">
         <v>268</v>
@@ -4985,16 +4985,16 @@
         <v>9</v>
       </c>
       <c r="W9" s="19" t="s">
+        <v>782</v>
+      </c>
+      <c r="X9" s="19" t="s">
         <v>783</v>
       </c>
-      <c r="X9" s="19" t="s">
+      <c r="Y9" s="19" t="s">
         <v>784</v>
       </c>
-      <c r="Y9" s="19" t="s">
-        <v>785</v>
-      </c>
       <c r="Z9" s="19" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="AA9" s="3">
         <v>9</v>
@@ -5220,13 +5220,13 @@
         <v>10</v>
       </c>
       <c r="W10" s="19" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="X10" s="19" t="s">
         <v>729</v>
       </c>
       <c r="Y10" s="19" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="Z10" s="19" t="s">
         <v>748</v>
@@ -5455,16 +5455,16 @@
         <v>11</v>
       </c>
       <c r="W11" s="19" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="X11" s="19" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="Y11" s="19" t="s">
+        <v>830</v>
+      </c>
+      <c r="Z11" s="19" t="s">
         <v>831</v>
-      </c>
-      <c r="Z11" s="19" t="s">
-        <v>832</v>
       </c>
       <c r="AA11" s="3">
         <v>11</v>
@@ -5690,16 +5690,16 @@
         <v>12</v>
       </c>
       <c r="W12" s="19" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="X12" s="19" t="s">
         <v>730</v>
       </c>
       <c r="Y12" s="19" t="s">
+        <v>789</v>
+      </c>
+      <c r="Z12" s="19" t="s">
         <v>790</v>
-      </c>
-      <c r="Z12" s="19" t="s">
-        <v>791</v>
       </c>
       <c r="AA12" s="3">
         <v>12</v>
@@ -5928,13 +5928,13 @@
         <v>756</v>
       </c>
       <c r="X13" s="19" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="Y13" s="19" t="s">
+        <v>832</v>
+      </c>
+      <c r="Z13" s="19" t="s">
         <v>833</v>
-      </c>
-      <c r="Z13" s="19" t="s">
-        <v>834</v>
       </c>
       <c r="AA13" s="3">
         <v>13</v>
@@ -5946,10 +5946,10 @@
         <v>441</v>
       </c>
       <c r="AD13" s="3" t="s">
+        <v>834</v>
+      </c>
+      <c r="AE13" s="3" t="s">
         <v>835</v>
-      </c>
-      <c r="AE13" s="3" t="s">
-        <v>836</v>
       </c>
       <c r="AF13" s="4" t="s">
         <v>236</v>
@@ -6163,13 +6163,13 @@
         <v>749</v>
       </c>
       <c r="X14" s="19" t="s">
+        <v>792</v>
+      </c>
+      <c r="Y14" s="19" t="s">
         <v>793</v>
       </c>
-      <c r="Y14" s="19" t="s">
+      <c r="Z14" s="19" t="s">
         <v>794</v>
-      </c>
-      <c r="Z14" s="19" t="s">
-        <v>795</v>
       </c>
       <c r="AA14" s="3">
         <v>14</v>
@@ -6395,16 +6395,16 @@
         <v>15</v>
       </c>
       <c r="W15" s="19" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="X15" s="19" t="s">
         <v>731</v>
       </c>
       <c r="Y15" s="19" t="s">
+        <v>796</v>
+      </c>
+      <c r="Z15" s="19" t="s">
         <v>797</v>
-      </c>
-      <c r="Z15" s="19" t="s">
-        <v>798</v>
       </c>
       <c r="AA15" s="3">
         <v>15</v>
@@ -6428,7 +6428,7 @@
         <v>3</v>
       </c>
       <c r="AH15" s="1" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="AI15" s="3" t="s">
         <v>305</v>
@@ -6630,10 +6630,10 @@
         <v>16</v>
       </c>
       <c r="W16" s="19" t="s">
+        <v>798</v>
+      </c>
+      <c r="X16" s="19" t="s">
         <v>799</v>
-      </c>
-      <c r="X16" s="19" t="s">
-        <v>800</v>
       </c>
       <c r="Y16" s="19" t="s">
         <v>695</v>
@@ -6865,16 +6865,16 @@
         <v>17</v>
       </c>
       <c r="W17" s="19" t="s">
+        <v>840</v>
+      </c>
+      <c r="X17" s="19" t="s">
         <v>841</v>
       </c>
-      <c r="X17" s="19" t="s">
-        <v>842</v>
-      </c>
       <c r="Y17" s="19" t="s">
+        <v>800</v>
+      </c>
+      <c r="Z17" s="19" t="s">
         <v>801</v>
-      </c>
-      <c r="Z17" s="19" t="s">
-        <v>802</v>
       </c>
       <c r="AA17" s="3">
         <v>17</v>
@@ -7100,10 +7100,10 @@
         <v>18</v>
       </c>
       <c r="W18" s="19" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="X18" s="19" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="Y18" s="19" t="s">
         <v>750</v>
@@ -7335,16 +7335,16 @@
         <v>19</v>
       </c>
       <c r="W19" s="19" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="X19" s="19" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="Y19" s="19" t="s">
         <v>752</v>
       </c>
       <c r="Z19" s="19" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="AA19" s="3">
         <v>19</v>
@@ -7570,16 +7570,16 @@
         <v>20</v>
       </c>
       <c r="W20" s="19" t="s">
+        <v>805</v>
+      </c>
+      <c r="X20" s="19" t="s">
         <v>806</v>
       </c>
-      <c r="X20" s="19" t="s">
+      <c r="Y20" s="19" t="s">
         <v>807</v>
       </c>
-      <c r="Y20" s="19" t="s">
+      <c r="Z20" s="19" t="s">
         <v>808</v>
-      </c>
-      <c r="Z20" s="19" t="s">
-        <v>809</v>
       </c>
       <c r="AA20" s="3">
         <v>20</v>
@@ -7805,10 +7805,10 @@
         <v>21</v>
       </c>
       <c r="W21" s="19" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="X21" s="19" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="Y21" s="19" t="s">
         <v>753</v>
@@ -8040,16 +8040,16 @@
         <v>22</v>
       </c>
       <c r="W22" s="19" t="s">
+        <v>810</v>
+      </c>
+      <c r="X22" s="19" t="s">
         <v>811</v>
       </c>
-      <c r="X22" s="19" t="s">
+      <c r="Y22" s="19" t="s">
         <v>812</v>
       </c>
-      <c r="Y22" s="19" t="s">
+      <c r="Z22" s="19" t="s">
         <v>813</v>
-      </c>
-      <c r="Z22" s="19" t="s">
-        <v>814</v>
       </c>
       <c r="AA22" s="3">
         <v>22</v>
@@ -8278,13 +8278,13 @@
         <v>737</v>
       </c>
       <c r="X23" s="19" t="s">
+        <v>814</v>
+      </c>
+      <c r="Y23" s="19" t="s">
         <v>815</v>
       </c>
-      <c r="Y23" s="19" t="s">
+      <c r="Z23" s="19" t="s">
         <v>816</v>
-      </c>
-      <c r="Z23" s="19" t="s">
-        <v>817</v>
       </c>
       <c r="AA23" s="3">
         <v>23</v>
@@ -8513,7 +8513,7 @@
         <v>738</v>
       </c>
       <c r="X24" s="19" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="Y24" s="19" t="s">
         <v>410</v>
@@ -8751,10 +8751,10 @@
         <v>740</v>
       </c>
       <c r="Y25" s="19" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="Z25" s="19" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="AA25">
         <v>25</v>
@@ -9845,7 +9845,7 @@
       </c>
       <c r="BP33" s="19" t="str">
         <f t="shared" si="53"/>
-        <v xml:space="preserve">The A67 highway the longest road in the county. It spanned almost all of it, and ran over the river Stig. Heading to Innsmouth from Ipswich people had to cross the bridge over the river. Somewhere before this bridge there was a rest stop that offered travellers refreshment. It was a popular place and saw a great many visitors, making it a profitable place to own. A checkpoint had been set up by the police somewhere before the rest stop as there had been reports of drug smuggling in the area. </v>
+        <v xml:space="preserve">The A67 highway was the longest road in the county. It spanned almost all of it, and ran over the river Stig. Heading to Innsmouth from Ipswich people had to cross the bridge over the river. Somewhere before this bridge there was a rest stop that offered travellers refreshment. It was a popular place and saw a great many visitors, making it a profitable place to own. A checkpoint had been set up by the police somewhere before the rest stop as there had been reports of drug smuggling in the area. </v>
       </c>
       <c r="BQ33" s="19" t="str">
         <f t="shared" si="54"/>
@@ -10729,11 +10729,11 @@
       </c>
       <c r="D43" s="3" t="str">
         <f ca="1">INDIRECT("Z"&amp;A43)</f>
-        <v xml:space="preserve">The A67 highway the longest road in the county. It spanned almost all of it, and ran over the river Stig. Heading to Innsmouth from Ipswich people had to cross the bridge over the river. Somewhere before this bridge there was a rest stop that offered travellers refreshment. It was a popular place and saw a great many visitors, making it a profitable place to own. A checkpoint had been set up by the police somewhere before the rest stop as there had been reports of drug smuggling in the area. </v>
+        <v xml:space="preserve">The A67 highway was the longest road in the county. It spanned almost all of it, and ran over the river Stig. Heading to Innsmouth from Ipswich people had to cross the bridge over the river. Somewhere before this bridge there was a rest stop that offered travellers refreshment. It was a popular place and saw a great many visitors, making it a profitable place to own. A checkpoint had been set up by the police somewhere before the rest stop as there had been reports of drug smuggling in the area. </v>
       </c>
       <c r="E43" s="3" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v xml:space="preserve">Harriet often travelled the long A67 highway. She had what she considered to be one of the most expensive cars in her neighbourhood, far more expensive than her neighbour Barry's car. Harriet was arrogant and boastful so it made her happy that he struggled to purchase his car whereas she could easily afford hers. Harriet's other neighbour Olive had an even less expensive car than Barry. Harriet enjoyed washing her car every weekend. The A67 highway the longest road in the county. It spanned almost all of it, and ran over the river Stig. Heading to Innsmouth from Ipswich people had to cross the bridge over the river. Somewhere before this bridge there was a rest stop that offered travellers refreshment. It was a popular place and saw a great many visitors, making it a profitable place to own. A checkpoint had been set up by the police somewhere before the rest stop as there had been reports of drug smuggling in the area. </v>
+        <v xml:space="preserve">Harriet often travelled the long A67 highway. She had what she considered to be one of the most expensive cars in her neighbourhood, far more expensive than her neighbour Barry's car. Harriet was arrogant and boastful so it made her happy that he struggled to purchase his car whereas she could easily afford hers. Harriet's other neighbour Olive had an even less expensive car than Barry. Harriet enjoyed washing her car every weekend. The A67 highway was the longest road in the county. It spanned almost all of it, and ran over the river Stig. Heading to Innsmouth from Ipswich people had to cross the bridge over the river. Somewhere before this bridge there was a rest stop that offered travellers refreshment. It was a popular place and saw a great many visitors, making it a profitable place to own. A checkpoint had been set up by the police somewhere before the rest stop as there had been reports of drug smuggling in the area. </v>
       </c>
       <c r="F43" s="3" t="str">
         <f ca="1">INDIRECT("AH"&amp;A43)</f>
@@ -10823,11 +10823,11 @@
       </c>
       <c r="D44" s="3" t="str">
         <f ca="1">INDIRECT("Z"&amp;A44)</f>
-        <v xml:space="preserve">The A67 highway the longest road in the county. It spanned almost all of it, and ran over the river Stig. Heading to Innsmouth from Ipswich people had to cross the bridge over the river. Somewhere before this bridge there was a rest stop that offered travellers refreshment. It was a popular place and saw a great many visitors, making it a profitable place to own. A checkpoint had been set up by the police somewhere before the rest stop as there had been reports of drug smuggling in the area. </v>
+        <v xml:space="preserve">The A67 highway was the longest road in the county. It spanned almost all of it, and ran over the river Stig. Heading to Innsmouth from Ipswich people had to cross the bridge over the river. Somewhere before this bridge there was a rest stop that offered travellers refreshment. It was a popular place and saw a great many visitors, making it a profitable place to own. A checkpoint had been set up by the police somewhere before the rest stop as there had been reports of drug smuggling in the area. </v>
       </c>
       <c r="E44" s="3" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v xml:space="preserve">Harriet often travelled the long A67 highway. She had what she considered to be one of the most expensive cars in her neighbourhood, far more expensive than her neighbour Barry's car. Harriet was arrogant and boastful so it made her happy that he struggled to purchase his car whereas she could easily afford hers. Harriet's other neighbour Olive had a much nicer and more expensive car than Barry. Harriet enjoyed washing her car every weekend. The A67 highway the longest road in the county. It spanned almost all of it, and ran over the river Stig. Heading to Innsmouth from Ipswich people had to cross the bridge over the river. Somewhere before this bridge there was a rest stop that offered travellers refreshment. It was a popular place and saw a great many visitors, making it a profitable place to own. A checkpoint had been set up by the police somewhere before the rest stop as there had been reports of drug smuggling in the area. </v>
+        <v xml:space="preserve">Harriet often travelled the long A67 highway. She had what she considered to be one of the most expensive cars in her neighbourhood, far more expensive than her neighbour Barry's car. Harriet was arrogant and boastful so it made her happy that he struggled to purchase his car whereas she could easily afford hers. Harriet's other neighbour Olive had a much nicer and more expensive car than Barry. Harriet enjoyed washing her car every weekend. The A67 highway was the longest road in the county. It spanned almost all of it, and ran over the river Stig. Heading to Innsmouth from Ipswich people had to cross the bridge over the river. Somewhere before this bridge there was a rest stop that offered travellers refreshment. It was a popular place and saw a great many visitors, making it a profitable place to own. A checkpoint had been set up by the police somewhere before the rest stop as there had been reports of drug smuggling in the area. </v>
       </c>
       <c r="F44" s="3" t="str">
         <f ca="1">INDIRECT("AH"&amp;A44)</f>
@@ -11101,7 +11101,7 @@
       </c>
       <c r="C47" s="3" t="str">
         <f ca="1">INDIRECT("Z"&amp;A47)</f>
-        <v xml:space="preserve">The A67 highway the longest road in the county. It spanned almost all of it, and ran over the river Stig. Heading to Innsmouth from Ipswich people had to cross the bridge over the river. Somewhere before this bridge there was a rest stop that offered travellers refreshment. It was a popular place and saw a great many visitors, making it a profitable place to own. A checkpoint had been set up by the police somewhere before the rest stop as there had been reports of drug smuggling in the area. </v>
+        <v xml:space="preserve">The A67 highway was the longest road in the county. It spanned almost all of it, and ran over the river Stig. Heading to Innsmouth from Ipswich people had to cross the bridge over the river. Somewhere before this bridge there was a rest stop that offered travellers refreshment. It was a popular place and saw a great many visitors, making it a profitable place to own. A checkpoint had been set up by the police somewhere before the rest stop as there had been reports of drug smuggling in the area. </v>
       </c>
       <c r="D47" s="3" t="str">
         <f ca="1">INDIRECT("X"&amp;A47)</f>
@@ -11109,7 +11109,7 @@
       </c>
       <c r="E47" s="3" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v xml:space="preserve">The A67 highway the longest road in the county. It spanned almost all of it, and ran over the river Stig. Heading to Innsmouth from Ipswich people had to cross the bridge over the river. Somewhere before this bridge there was a rest stop that offered travellers refreshment. It was a popular place and saw a great many visitors, making it a profitable place to own. A checkpoint had been set up by the police somewhere before the rest stop as there had been reports of drug smuggling in the area. Harriet often travelled the long A67 highway. She had what she considered to be one of the most expensive cars in her neighbourhood, far more expensive than her neighbour Barry's car. Harriet was arrogant and boastful so it made her happy that he struggled to purchase his car whereas she could easily afford hers. Harriet's other neighbour Olive had an even less expensive car than Barry. Harriet enjoyed washing her car every weekend. </v>
+        <v xml:space="preserve">The A67 highway was the longest road in the county. It spanned almost all of it, and ran over the river Stig. Heading to Innsmouth from Ipswich people had to cross the bridge over the river. Somewhere before this bridge there was a rest stop that offered travellers refreshment. It was a popular place and saw a great many visitors, making it a profitable place to own. A checkpoint had been set up by the police somewhere before the rest stop as there had been reports of drug smuggling in the area. Harriet often travelled the long A67 highway. She had what she considered to be one of the most expensive cars in her neighbourhood, far more expensive than her neighbour Barry's car. Harriet was arrogant and boastful so it made her happy that he struggled to purchase his car whereas she could easily afford hers. Harriet's other neighbour Olive had an even less expensive car than Barry. Harriet enjoyed washing her car every weekend. </v>
       </c>
       <c r="F47" s="3" t="str">
         <f ca="1">INDIRECT("AC"&amp;A47)</f>
@@ -11289,7 +11289,7 @@
       </c>
       <c r="C49" s="3" t="str">
         <f ca="1">INDIRECT("Z"&amp;A49)</f>
-        <v xml:space="preserve">The A67 highway the longest road in the county. It spanned almost all of it, and ran over the river Stig. Heading to Innsmouth from Ipswich people had to cross the bridge over the river. Somewhere before this bridge there was a rest stop that offered travellers refreshment. It was a popular place and saw a great many visitors, making it a profitable place to own. A checkpoint had been set up by the police somewhere before the rest stop as there had been reports of drug smuggling in the area. </v>
+        <v xml:space="preserve">The A67 highway was the longest road in the county. It spanned almost all of it, and ran over the river Stig. Heading to Innsmouth from Ipswich people had to cross the bridge over the river. Somewhere before this bridge there was a rest stop that offered travellers refreshment. It was a popular place and saw a great many visitors, making it a profitable place to own. A checkpoint had been set up by the police somewhere before the rest stop as there had been reports of drug smuggling in the area. </v>
       </c>
       <c r="D49" s="3" t="str">
         <f ca="1">INDIRECT("W"&amp;A49)</f>
@@ -11297,7 +11297,7 @@
       </c>
       <c r="E49" s="3" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v xml:space="preserve">The A67 highway the longest road in the county. It spanned almost all of it, and ran over the river Stig. Heading to Innsmouth from Ipswich people had to cross the bridge over the river. Somewhere before this bridge there was a rest stop that offered travellers refreshment. It was a popular place and saw a great many visitors, making it a profitable place to own. A checkpoint had been set up by the police somewhere before the rest stop as there had been reports of drug smuggling in the area. Harriet often travelled the long A67 highway. She had what she considered to be one of the most expensive cars in her neighbourhood, far more expensive than her neighbour Barry's car. Harriet was arrogant and boastful so it made her happy that he struggled to purchase his car whereas she could easily afford hers. Harriet's other neighbour Olive had a much nicer and more expensive car than Barry. Harriet enjoyed washing her car every weekend. </v>
+        <v xml:space="preserve">The A67 highway was the longest road in the county. It spanned almost all of it, and ran over the river Stig. Heading to Innsmouth from Ipswich people had to cross the bridge over the river. Somewhere before this bridge there was a rest stop that offered travellers refreshment. It was a popular place and saw a great many visitors, making it a profitable place to own. A checkpoint had been set up by the police somewhere before the rest stop as there had been reports of drug smuggling in the area. Harriet often travelled the long A67 highway. She had what she considered to be one of the most expensive cars in her neighbourhood, far more expensive than her neighbour Barry's car. Harriet was arrogant and boastful so it made her happy that he struggled to purchase his car whereas she could easily afford hers. Harriet's other neighbour Olive had a much nicer and more expensive car than Barry. Harriet enjoyed washing her car every weekend. </v>
       </c>
       <c r="F49" s="3" t="str">
         <f ca="1">INDIRECT("AC"&amp;A49)</f>

</xml_diff>